<commit_message>
implemented mixed languages on activity executions
</commit_message>
<xml_diff>
--- a/public/activity_execution_upload_template.xlsx
+++ b/public/activity_execution_upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sihu/p/bula/mova21-orca/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\james\mova21-orca\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9CC4B7-7F5B-A242-90C9-F7E1CD7FF9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED57F1D-5B45-4203-95CF-167558DEB372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{751C7588-BA65-2943-84B1-AD9DF869C175}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{751C7588-BA65-2943-84B1-AD9DF869C175}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Startzeit</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Feld 2</t>
+  </si>
+  <si>
+    <t>Gemischte Durchfuehrung</t>
   </si>
 </sst>
 </file>
@@ -434,22 +437,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C17ADCD-4EA4-1741-9059-31CB93874788}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.1875" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +474,11 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>44765.6875</v>
       </c>
@@ -494,8 +500,11 @@
       <c r="G2" t="s">
         <v>6</v>
       </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
         <v>44765.729166666664</v>
       </c>
@@ -517,8 +526,11 @@
       <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>

</xml_diff>

<commit_message>
Add Transport-IDs on Activity Executions
</commit_message>
<xml_diff>
--- a/public/activity_execution_upload_template.xlsx
+++ b/public/activity_execution_upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\james\mova21-orca\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sihu/p/bula/mova21-orca/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED57F1D-5B45-4203-95CF-167558DEB372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF00498-4917-004D-92DE-6E13352703F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{751C7588-BA65-2943-84B1-AD9DF869C175}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29000" windowHeight="15800" xr2:uid="{751C7588-BA65-2943-84B1-AD9DF869C175}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Startzeit</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Gemischte Durchfuehrung</t>
+  </si>
+  <si>
+    <t>Transport IDS (falls mit Transport) (kommagetrennt)</t>
   </si>
 </sst>
 </file>
@@ -437,22 +440,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C17ADCD-4EA4-1741-9059-31CB93874788}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="13.1875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.1875" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.1640625" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="9" max="9" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,8 +481,11 @@
       <c r="H1" t="s">
         <v>13</v>
       </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44765.6875</v>
       </c>
@@ -504,7 +511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44765.729166666664</v>
       </c>
@@ -530,7 +537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>

</xml_diff>